<commit_message>
Open access permissions on Test Plan
</commit_message>
<xml_diff>
--- a/docs/Caliptra_Gen2_SS_TestPlan.xlsx
+++ b/docs/Caliptra_Gen2_SS_TestPlan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cwhitehead\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:101_{756EFBF9-FC2B-44CA-94DB-9AB1533EE1DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:101_{DDB43A5E-9C5C-4098-AD26-4DAFF72EF89F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{9B473A9E-6712-4ADB-AA20-757BC467C8BB}"/>
   </bookViews>
@@ -1274,7 +1274,7 @@
   <dimension ref="A1:C183"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A154" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="M170" sqref="M170"/>
     </sheetView>
   </sheetViews>

</xml_diff>